<commit_message>
add color and order num
</commit_message>
<xml_diff>
--- a/doorcalculate/polls/document_gen/to_excel.xlsx
+++ b/doorcalculate/polls/document_gen/to_excel.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,139 +429,139 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Тип короба</t>
+          <t>Тип коробу</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Открывание</t>
+          <t>Відкривання</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Сторона</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Сторона</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>Полотно</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Короб</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Проем</t>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Отвір</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Оздоблення полотна</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Отделки полотна</t>
+          <t>Алюм обв'язок</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Алюм обвяз</t>
+          <t>Колір фарбування профілю</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Цвет покраски профиля</t>
+          <t>Колір ущільнювача</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Цвет уплотнителя</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Сторона</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Врезка</t>
+          <t>Врізання</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Колір фурн</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>к-сть</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>колво</t>
+          <t>Ціна</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>Цена</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>Всего</t>
+          <t>Усього</t>
         </is>
       </c>
     </row>
     <row r="2">
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Отвори</t>
+        </is>
+      </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Отверствия</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Петли</t>
+          <t>Петлі</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ширина мм обличчя\тил</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ширина мм лицо\тыл</t>
+          <t>Висота мм обличчя\тил</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Высота мм лицо\тыл</t>
+          <t>Ширина мм</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>Висота мм</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>Ширина мм</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Высота мм</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Ширина мм</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Высота мм</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>ручка</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
+          <t>Висота мм</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Ручка</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>WC/PZ</t>
         </is>
       </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>грн</t>
+        </is>
+      </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>грн</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
         <is>
           <t>грн</t>
         </is>
@@ -570,12 +570,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Multistrato</t>
+          <t>Grezza PN ґрунт</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Slim Light</t>
+          <t>SlimTS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,190 +585,217 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Наружное</t>
+          <t>лицьова</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>лицо</t>
+          <t>615</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>2100</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>689</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>672</t>
+          <t>2145</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2034</t>
+          <t>669</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>652</t>
+          <t>2135</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>Ґрунт</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Ламинатин</t>
+          <t>+</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Чорний</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Аннодированый</t>
+          <t>Чорний</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Серый</t>
+          <t>+</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>лицо</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>2</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>WC</t>
+          <t>Чорний</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15990</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>10980</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>10980</t>
+          <t>79950</t>
         </is>
       </c>
     </row>
     <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Зовнішнє</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>тил</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>тыл</t>
+          <t>593</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>620</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>тыл</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>WC</t>
+          <t>2089</t>
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Усього за дверні блоки: 79950.0 грн
+		Знижка:0.0%
+		Усього, з урахуванням знижки: 79950.0 грн
+		Доставка на склад (об'єкт) без вивантаження та занесення на поверх: 0.0 грн
+		Монтаж:500.0грнЗаміри: 0.0 грн
+		Всього за послуги: 2500.0 грн
+		Підсумки без ПДВ: 82450.0 грн
+		Передплата: 0.0 % 
+		Передплата: 0.0 грн 
+		Залишок: 82450.0 грн</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Місто: Замовник: 
+		Доставка замовлення: 
+		Контакти: 
+		Ел.Адреса:</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Висота ручки: 1000 мм. від низу полотна.
+			Зазор від підлоги до полотна: 8 мм.
+			Без вартості ручок.
+			Термін виготовлення: 1-4 тижнів з моменту погодження та внесення передоплати.
+			Примітка:</t>
+        </is>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
   </sheetData>
   <mergeCells count="56">
     <mergeCell ref="N1:N3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="G4"/>
-    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R4:R5"/>
     <mergeCell ref="T4:T5"/>
-    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="P3"/>
     <mergeCell ref="H3"/>
     <mergeCell ref="J3"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="P5"/>
-    <mergeCell ref="R5"/>
-    <mergeCell ref="K3"/>
+    <mergeCell ref="D5"/>
+    <mergeCell ref="A9:G18"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="T3"/>
     <mergeCell ref="F4"/>
-    <mergeCell ref="V3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="Q3"/>
+    <mergeCell ref="O3"/>
+    <mergeCell ref="E3"/>
     <mergeCell ref="J4:J5"/>
-    <mergeCell ref="P4"/>
+    <mergeCell ref="G1:H2"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="C5"/>
+    <mergeCell ref="T1:T2"/>
     <mergeCell ref="E5"/>
+    <mergeCell ref="O9:U18"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="R4"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="C4"/>
+    <mergeCell ref="H9:N18"/>
+    <mergeCell ref="K1:K3"/>
     <mergeCell ref="E4"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="F3"/>
-    <mergeCell ref="F1:G2"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="H1:I2"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J1:K2"/>
     <mergeCell ref="S4:S5"/>
+    <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="U4:U5"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="Q5"/>
     <mergeCell ref="F5"/>
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="Q4"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C1:C3"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="G3"/>
     <mergeCell ref="I3"/>
     <mergeCell ref="H4:H5"/>
+    <mergeCell ref="E1:F2"/>
     <mergeCell ref="U3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="R3"/>
     <mergeCell ref="N4:N5"/>
-    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="L1:L3"/>
-    <mergeCell ref="G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
correct path for files
</commit_message>
<xml_diff>
--- a/doorcalculate/polls/document_gen/to_excel.xlsx
+++ b/doorcalculate/polls/document_gen/to_excel.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,12 +518,12 @@
     <row r="3">
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ширина мм обличчя\тил</t>
+          <t>Ширина мм лице\тил</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Висота мм обличчя\тил</t>
+          <t>Висота мм лице\тил</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -567,151 +567,22 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Grezza PN ґрунт</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SlimTS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Левое</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>лицьова</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>615</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2100</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>689</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2145</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>669</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2135</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Ґрунт</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Чорний</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Чорний</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>WC</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Чорний</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>15990</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>79950</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Зовнішнє</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>тил</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>593</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2089</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Усього за дверні блоки: 79950.0 грн
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Всього за дверні блоки: 0.0 грн
 		Знижка:0.0%
-		Усього, з урахуванням знижки: 79950.0 грн
+		Усього, з урахуванням знижки: 0.0 грн
 		Доставка на склад (об'єкт) без вивантаження та занесення на поверх: 0.0 грн
-		Монтаж:500.0грнЗаміри: 0.0 грн
-		Всього за послуги: 2500.0 грн
-		Підсумки без ПДВ: 82450.0 грн
+		Монтаж:0.0грнЗаміри: 0.0 грн
+		Всього за послуги: 0.0 грн
+		Всього сума замовлення: 0.0 грн
 		Передплата: 0.0 % 
 		Передплата: 0.0 грн 
-		Залишок: 82450.0 грн</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
+		Залишок: 0.0 грн</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Місто: Замовник: 
 		Доставка замовлення: 
@@ -719,7 +590,7 @@
 		Ел.Адреса:</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>Висота ручки: 1000 мм. від низу полотна.
 			Зазор від підлоги до полотна: 8 мм.
@@ -729,6 +600,8 @@
         </is>
       </c>
     </row>
+    <row r="8"/>
+    <row r="9"/>
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>
@@ -736,65 +609,38 @@
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="31">
     <mergeCell ref="N1:N3"/>
-    <mergeCell ref="D4"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="T4:T5"/>
     <mergeCell ref="P3"/>
     <mergeCell ref="H3"/>
     <mergeCell ref="J3"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="D5"/>
-    <mergeCell ref="A9:G18"/>
+    <mergeCell ref="O7:U16"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="T3"/>
-    <mergeCell ref="F4"/>
     <mergeCell ref="O3"/>
     <mergeCell ref="E3"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="G1:H2"/>
-    <mergeCell ref="L4:L5"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="S1:S3"/>
-    <mergeCell ref="C5"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="E5"/>
-    <mergeCell ref="O9:U18"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="R1:R3"/>
-    <mergeCell ref="C4"/>
-    <mergeCell ref="H9:N18"/>
     <mergeCell ref="K1:K3"/>
-    <mergeCell ref="E4"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="G4:G5"/>
     <mergeCell ref="F3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="A7:G16"/>
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="F5"/>
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="M4:M5"/>
     <mergeCell ref="G3"/>
     <mergeCell ref="I3"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="E1:F2"/>
     <mergeCell ref="U3"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="H7:N16"/>
     <mergeCell ref="L1:L3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>